<commit_message>
screen lock during game
</commit_message>
<xml_diff>
--- a/map-maker.xlsx
+++ b/map-maker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c9f0e370f672401/Bureau/Ironhack/projects/gaming-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF247369-910D-427C-99E5-4B1D0330E0D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{CF247369-910D-427C-99E5-4B1D0330E0D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68FAD421-410A-4D9A-BA0B-22454A204BEC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A4924E79-6CC4-407B-ABAB-BE2287AD5D6C}"/>
+    <workbookView xWindow="-27270" yWindow="2010" windowWidth="26745" windowHeight="12270" xr2:uid="{A4924E79-6CC4-407B-ABAB-BE2287AD5D6C}"/>
   </bookViews>
   <sheets>
     <sheet name="DIAMOND" sheetId="1" r:id="rId1"/>
@@ -125,6 +125,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,20 +444,20 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>1</v>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>0</v>
@@ -467,20 +471,20 @@
       <c r="L1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>1</v>
+      <c r="M1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>0</v>
@@ -493,7 +497,7 @@
       </c>
       <c r="U1" t="str">
         <f>_xlfn.CONCAT("["&amp;_xlfn.CONCAT(A1:T1)&amp;"]")&amp;","</f>
-        <v>['0','0','0','B','B','B','B','B','0','0','0','0','B','B','B','B','B','0','0','0',],</v>
+        <v>['0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0',],</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -509,14 +513,14 @@
       <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>1</v>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>0</v>
@@ -536,14 +540,14 @@
       <c r="M2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>1</v>
+      <c r="N2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>0</v>
@@ -559,7 +563,7 @@
       </c>
       <c r="U2" t="str">
         <f t="shared" ref="U2:U20" si="0">_xlfn.CONCAT("["&amp;_xlfn.CONCAT(A2:T2)&amp;"]")&amp;","</f>
-        <v>['0','0','0','0','B','B','B','0','0','0','0','0','0','B','B','B','0','0','0','0',],</v>
+        <v>['0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0',],</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -578,8 +582,8 @@
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>1</v>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>0</v>
@@ -605,8 +609,8 @@
       <c r="N3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>1</v>
+      <c r="O3" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>0</v>
@@ -625,7 +629,7 @@
       </c>
       <c r="U3" t="str">
         <f t="shared" si="0"/>
-        <v>['0','0','0','0','0','B','0','0','0','0','0','0','0','0','B','0','0','0','0','0',],</v>
+        <v>['0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0',],</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -635,53 +639,53 @@
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>0</v>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>0</v>
@@ -691,7 +695,7 @@
       </c>
       <c r="U4" t="str">
         <f t="shared" si="0"/>
-        <v>['0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0',],</v>
+        <v>['0','0','W','W','W','W','W','W','W','W','W','W','W','W','W','W','W','W','0','0',],</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -722,11 +726,11 @@
       <c r="I5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>1</v>
+      <c r="J5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>0</v>
@@ -757,7 +761,7 @@
       </c>
       <c r="U5" t="str">
         <f t="shared" si="0"/>
-        <v>['0','0','0','0','0','0','0','0','0','B','B','0','0','0','0','0','0','0','0','0',],</v>
+        <v>['0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0',],</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -785,17 +789,17 @@
       <c r="H6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>1</v>
+      <c r="I6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>0</v>
@@ -823,7 +827,7 @@
       </c>
       <c r="U6" t="str">
         <f t="shared" si="0"/>
-        <v>['0','0','0','0','0','0','0','0','B','B','B','B','0','0','0','0','0','0','0','0',],</v>
+        <v>['0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0',],</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -833,20 +837,20 @@
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>0</v>
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>1</v>
@@ -866,20 +870,20 @@
       <c r="M7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>0</v>
+      <c r="N7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>0</v>
@@ -889,7 +893,7 @@
       </c>
       <c r="U7" t="str">
         <f t="shared" si="0"/>
-        <v>['0','0','0','0','0','0','0','B','B','B','B','B','B','0','0','0','0','0','0','0',],</v>
+        <v>['0','0','B','B','B','B','B','B','B','B','B','B','B','B','B','B','B','B','0','0',],</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -899,17 +903,17 @@
       <c r="B8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>0</v>
+      <c r="C8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>1</v>
@@ -920,11 +924,11 @@
       <c r="I8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>2</v>
+      <c r="J8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>1</v>
@@ -935,17 +939,17 @@
       <c r="N8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>0</v>
+      <c r="O8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>0</v>
@@ -955,7 +959,7 @@
       </c>
       <c r="U8" t="str">
         <f t="shared" si="0"/>
-        <v>['0','0','0','0','0','0','B','B','B','W','W','B','B','B','0','0','0','0','0','0',],</v>
+        <v>['0','0','B','B','B','B','B','B','B','B','B','B','B','B','B','B','B','B','0','0',],</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -974,35 +978,35 @@
       <c r="E9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>1</v>
+      <c r="F9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="P9" s="1" t="s">
         <v>0</v>
@@ -1021,7 +1025,7 @@
       </c>
       <c r="U9" t="str">
         <f t="shared" si="0"/>
-        <v>['0','0','0','0','0','B','B','B','W','W','W','W','B','B','B','0','0','0','0','0',],</v>
+        <v>['0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0',],</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -1037,41 +1041,41 @@
       <c r="D10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>1</v>
+      <c r="E10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="Q10" s="1" t="s">
         <v>0</v>
@@ -1087,7 +1091,7 @@
       </c>
       <c r="U10" t="str">
         <f t="shared" si="0"/>
-        <v>['0','0','0','0','B','B','B','W','W','W','W','W','W','B','B','B','0','0','0','0',],</v>
+        <v>['0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0',],</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -1097,20 +1101,20 @@
       <c r="B11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>1</v>
+      <c r="C11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>2</v>
@@ -1130,20 +1134,20 @@
       <c r="M11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="N11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>0</v>
+      <c r="N11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="S11" s="1" t="s">
         <v>0</v>
@@ -1153,7 +1157,7 @@
       </c>
       <c r="U11" t="str">
         <f t="shared" si="0"/>
-        <v>['0','0','0','0','B','B','B','W','W','W','W','W','W','B','B','B','0','0','0','0',],</v>
+        <v>['0','0','W','W','W','W','W','W','W','W','W','W','W','W','W','W','W','W','0','0',],</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -1172,35 +1176,35 @@
       <c r="E12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O12" s="2" t="s">
-        <v>1</v>
+      <c r="F12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>0</v>
@@ -1219,7 +1223,7 @@
       </c>
       <c r="U12" t="str">
         <f t="shared" si="0"/>
-        <v>['0','0','0','0','0','B','B','B','W','W','W','W','B','B','B','0','0','0','0','0',],</v>
+        <v>['0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0',],</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -1241,29 +1245,29 @@
       <c r="F13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>1</v>
+      <c r="G13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>0</v>
@@ -1285,7 +1289,7 @@
       </c>
       <c r="U13" t="str">
         <f t="shared" si="0"/>
-        <v>['0','0','0','0','0','0','B','B','B','W','W','B','B','B','0','0','0','0','0','0',],</v>
+        <v>['0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0',],</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -1295,20 +1299,20 @@
       <c r="B14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>0</v>
+      <c r="C14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>1</v>
@@ -1328,20 +1332,20 @@
       <c r="M14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>0</v>
+      <c r="N14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="S14" s="1" t="s">
         <v>0</v>
@@ -1351,7 +1355,7 @@
       </c>
       <c r="U14" t="str">
         <f t="shared" si="0"/>
-        <v>['0','0','0','0','0','0','0','B','B','B','B','B','B','0','0','0','0','0','0','0',],</v>
+        <v>['0','0','B','B','B','B','B','B','B','B','B','B','B','B','B','B','B','B','0','0',],</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -1361,23 +1365,23 @@
       <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>0</v>
+      <c r="C15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>1</v>
@@ -1391,23 +1395,23 @@
       <c r="L15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>0</v>
+      <c r="M15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="S15" s="1" t="s">
         <v>0</v>
@@ -1417,7 +1421,7 @@
       </c>
       <c r="U15" t="str">
         <f t="shared" si="0"/>
-        <v>['0','0','0','0','0','0','0','0','B','B','B','B','0','0','0','0','0','0','0','0',],</v>
+        <v>['0','0','B','B','B','B','B','B','B','B','B','B','B','B','B','B','B','B','0','0',],</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -1448,11 +1452,11 @@
       <c r="I16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>1</v>
+      <c r="J16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>0</v>
@@ -1483,7 +1487,7 @@
       </c>
       <c r="U16" t="str">
         <f t="shared" si="0"/>
-        <v>['0','0','0','0','0','0','0','0','0','B','B','0','0','0','0','0','0','0','0','0',],</v>
+        <v>['0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0',],</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -1559,53 +1563,53 @@
       <c r="B18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>0</v>
+      <c r="C18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="S18" s="1" t="s">
         <v>0</v>
@@ -1615,7 +1619,7 @@
       </c>
       <c r="U18" t="str">
         <f t="shared" si="0"/>
-        <v>['0','0','0','0','0','B','0','0','0','0','0','0','0','0','B','0','0','0','0','0',],</v>
+        <v>['0','0','W','W','W','W','W','W','W','W','W','W','W','W','W','W','W','W','0','0',],</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -1631,14 +1635,14 @@
       <c r="D19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>1</v>
+      <c r="E19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>0</v>
@@ -1658,14 +1662,14 @@
       <c r="M19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>1</v>
+      <c r="N19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>0</v>
@@ -1681,7 +1685,7 @@
       </c>
       <c r="U19" t="str">
         <f t="shared" si="0"/>
-        <v>['0','0','0','0','B','B','B','0','0','0','0','0','0','B','B','B','0','0','0','0',],</v>
+        <v>['0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0',],</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -1694,20 +1698,20 @@
       <c r="C20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>1</v>
+      <c r="D20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>0</v>
@@ -1721,20 +1725,20 @@
       <c r="L20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>1</v>
+      <c r="M20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="R20" s="1" t="s">
         <v>0</v>
@@ -1747,10 +1751,11 @@
       </c>
       <c r="U20" t="str">
         <f t="shared" si="0"/>
-        <v>['0','0','0','B','B','B','B','B','0','0','0','0','B','B','B','B','B','0','0','0',],</v>
+        <v>['0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0','0',],</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>